<commit_message>
Mapping de la partie corps entre ML/CDA/FHIR 61528f199dc8d9a9ac67fbcfafd3eda85315b1e5
</commit_message>
<xml_diff>
--- a/mappingCorps/ig/StructureDefinition-fr-lm-accidents-transfusionnels.xlsx
+++ b/mappingCorps/ig/StructureDefinition-fr-lm-accidents-transfusionnels.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-07T21:00:10+00:00</t>
+    <t>2026-01-14T15:34:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Entrée Accident transfusionnel</t>
+    <t>Accident transfusionnel</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>